<commit_message>
Contribuindo para o TCC
</commit_message>
<xml_diff>
--- a/Reports/fichamentoTcc2019.xlsx
+++ b/Reports/fichamentoTcc2019.xlsx
@@ -176,16 +176,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -234,7 +235,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -243,11 +247,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,7 +533,7 @@
   <dimension ref="E2:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:G16"/>
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,32 +544,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="5:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
@@ -582,66 +583,66 @@
       </c>
     </row>
     <row r="7" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="9"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="9"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="9"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="9"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="9"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="9"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="9"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="5:7" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Up att fichamentoTcc2019 by: Robert
</commit_message>
<xml_diff>
--- a/Reports/fichamentoTcc2019.xlsx
+++ b/Reports/fichamentoTcc2019.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Referência</t>
   </si>
@@ -147,12 +147,6 @@
       </rPr>
       <t>Engenharia de Software</t>
     </r>
-  </si>
-  <si>
-    <t>pg 50.</t>
-  </si>
-  <si>
-    <t>pg 80</t>
   </si>
 </sst>
 </file>
@@ -241,14 +235,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:H7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,32 +538,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="5:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
@@ -583,9 +577,7 @@
       </c>
     </row>
     <row r="7" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
@@ -626,18 +618,16 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="5:8" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="5:7" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="6"/>

</xml_diff>